<commit_message>
feat: Implementa melhorias de status, notificaÃ§Ãµes e relatÃ³rios
- Corrige exibiÃ§Ã£o de status das entregas (Entregue/Atrasada/Pendente)
- Adiciona notificaÃ§Ãµes de entregas atrasadas para admins
- Implementa cÃ¡lculo de dias de atraso nas entregas
- Adiciona informaÃ§Ãµes do aprovador nos relatÃ³rios
- Corrige cards da pÃ¡gina de relatÃ³rios para mostrar entregas atrasadas
- Adiciona bolinhas coloridas de status nos cards de aprovaÃ§Ãµes
- Melhora exibiÃ§Ã£o de empresa e CNPJ nos cards e detalhes
- Atualiza Dashboard para refletir entregas atrasadas
- Adiciona comando para verificar entregas atrasadas
- Corrige problemas de timezone nas datas
- Atualiza templates de importaÃ§Ã£o em massa
- Adiciona documentaÃ§Ã£o completa das melhorias
</commit_message>
<xml_diff>
--- a/backend/media/templates/template_empresas.xlsx
+++ b/backend/media/templates/template_empresas.xlsx
@@ -9,7 +9,9 @@
   <sheets>
     <sheet name="Empresas" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Empresas'!$A$1:$H$1</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -26,12 +28,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
-      <color theme="1"/>
+      <color rgb="00FFFFFF"/>
       <sz val="11"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -43,7 +42,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCCCCC"/>
+        <fgColor rgb="00366092"/>
+        <bgColor rgb="00366092"/>
       </patternFill>
     </fill>
   </fills>
@@ -61,7 +61,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -427,135 +429,111 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="40" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="40" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Nome da Empresa</t>
+          <t>Codigo</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Razao Social</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>CNPJ</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Nome Fantasia</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>E-mail</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Telefone</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Endereço</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Responsável</t>
+          <t>Endereco</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Responsavel</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>EMP001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Empresa Exemplo Ltda</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>12.345.678/0001-90</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Exemplo Corp</t>
+          <t>12345678000190</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>Exemplo</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>contato@exemplo.com</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>(11) 99999-9999</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Rua Exemplo, 123</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>João Silva</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Outra Empresa S.A.</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>98.765.432/0001-10</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Outra Corp</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>contato@outra.com</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>(11) 88888-8888</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Av. Outra, 456</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Maria Santos</t>
+          <t>Rua Exemplo, 123 - Sao Paulo - SP</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Joao Silva</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>